<commit_message>
Fix examples for theses import
</commit_message>
<xml_diff>
--- a/django/apps/thesis/static/thesis/import-example.xlsx
+++ b/django/apps/thesis/static/thesis/import-example.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">kub36135</t>
   </si>
   <si>
-    <t xml:space="preserve">SE</t>
+    <t xml:space="preserve">EL</t>
   </si>
   <si>
     <t xml:space="preserve">Simulace OFDM signálu a analýza šíření ve vnitřních prostorách </t>
@@ -82,23 +82,7 @@
     <t xml:space="preserve">Ing. Eva Štýbnarová</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ste38068, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ros36243</t>
-    </r>
+    <t xml:space="preserve">ste38068, ros36243</t>
   </si>
   <si>
     <t xml:space="preserve">Ve</t>
@@ -173,23 +157,7 @@
     <t xml:space="preserve">kolar</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">okl37179, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">log39122</t>
-    </r>
+    <t xml:space="preserve">okl37179, log39122</t>
   </si>
   <si>
     <t xml:space="preserve">Priming, impulzivita, pracovní pamět: efekt vystavení evolučně významným stimulům na kognitivní procesy </t>
@@ -206,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -233,11 +201,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -319,10 +282,10 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="126.87"/>

</xml_diff>